<commit_message>
loaded newer dataset, reran analysis; fixed df copies in func
</commit_message>
<xml_diff>
--- a/data_output/summary_tables.xlsx
+++ b/data_output/summary_tables.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="17">
   <si>
     <t>Age_Group</t>
   </si>
@@ -432,7 +432,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -460,10 +460,10 @@
         <v>13</v>
       </c>
       <c r="C2">
-        <v>58</v>
+        <v>358</v>
       </c>
       <c r="D2">
-        <v>0.8829349977165474</v>
+        <v>2.154160900174499</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -474,10 +474,10 @@
         <v>14</v>
       </c>
       <c r="C3">
-        <v>239</v>
+        <v>1459</v>
       </c>
       <c r="D3">
-        <v>3.638301111280256</v>
+        <v>8.779108249593838</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -488,10 +488,10 @@
         <v>13</v>
       </c>
       <c r="C4">
-        <v>67</v>
+        <v>395</v>
       </c>
       <c r="D4">
-        <v>1.019942152534632</v>
+        <v>2.376797641253986</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -502,10 +502,10 @@
         <v>14</v>
       </c>
       <c r="C5">
-        <v>413</v>
+        <v>1284</v>
       </c>
       <c r="D5">
-        <v>6.287106104429897</v>
+        <v>7.726096636380047</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -516,10 +516,10 @@
         <v>13</v>
       </c>
       <c r="C6">
-        <v>161</v>
+        <v>544</v>
       </c>
       <c r="D6">
-        <v>2.45090576952352</v>
+        <v>3.2733618147903</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -530,10 +530,10 @@
         <v>14</v>
       </c>
       <c r="C7">
-        <v>681</v>
+        <v>1868</v>
       </c>
       <c r="D7">
-        <v>10.36687471456843</v>
+        <v>11.24014681990493</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -544,10 +544,10 @@
         <v>13</v>
       </c>
       <c r="C8">
-        <v>243</v>
+        <v>772</v>
       </c>
       <c r="D8">
-        <v>3.699193180088293</v>
+        <v>4.645285516577411</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -558,10 +558,10 @@
         <v>14</v>
       </c>
       <c r="C9">
-        <v>1120</v>
+        <v>2754</v>
       </c>
       <c r="D9">
-        <v>17.04977926625057</v>
+        <v>16.57139418737589</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -572,10 +572,10 @@
         <v>13</v>
       </c>
       <c r="C10">
-        <v>343</v>
+        <v>761</v>
       </c>
       <c r="D10">
-        <v>5.221494900289237</v>
+        <v>4.579096215175402</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -586,10 +586,10 @@
         <v>14</v>
       </c>
       <c r="C11">
-        <v>1532</v>
+        <v>3018</v>
       </c>
       <c r="D11">
-        <v>23.32166235347846</v>
+        <v>18.15993742102413</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -600,10 +600,10 @@
         <v>13</v>
       </c>
       <c r="C12">
-        <v>242</v>
+        <v>493</v>
       </c>
       <c r="D12">
-        <v>3.683970162886284</v>
+        <v>2.96648414465371</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -614,10 +614,10 @@
         <v>14</v>
       </c>
       <c r="C13">
-        <v>1158</v>
+        <v>2106</v>
       </c>
       <c r="D13">
-        <v>17.62825391992693</v>
+        <v>12.67224261387568</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -628,10 +628,10 @@
         <v>13</v>
       </c>
       <c r="C14">
-        <v>65</v>
+        <v>115</v>
       </c>
       <c r="D14">
-        <v>0.9894961181306134</v>
+        <v>0.6919790601119201</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -642,10 +642,10 @@
         <v>14</v>
       </c>
       <c r="C15">
-        <v>226</v>
+        <v>437</v>
       </c>
       <c r="D15">
-        <v>3.440401887654133</v>
+        <v>2.629520428425296</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -656,10 +656,10 @@
         <v>13</v>
       </c>
       <c r="C16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D16">
-        <v>0.04566905160602831</v>
+        <v>0.02406883687345809</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -670,10 +670,10 @@
         <v>14</v>
       </c>
       <c r="C17">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D17">
-        <v>0.137007154818085</v>
+        <v>0.1323786028040195</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -681,13 +681,27 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18">
         <v>9</v>
       </c>
       <c r="D18">
-        <v>0.137007154818085</v>
+        <v>0.0541548829652807</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19">
+        <v>220</v>
+      </c>
+      <c r="D19">
+        <v>1.323786028040195</v>
       </c>
     </row>
   </sheetData>
@@ -731,10 +745,10 @@
         <v>13</v>
       </c>
       <c r="D2">
-        <v>469</v>
+        <v>1967</v>
       </c>
       <c r="E2">
-        <v>7.139595067742427</v>
+        <v>11.83585053252302</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -748,10 +762,10 @@
         <v>14</v>
       </c>
       <c r="D3">
-        <v>148</v>
+        <v>412</v>
       </c>
       <c r="E3">
-        <v>2.253006545897397</v>
+        <v>2.479090197966183</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -765,10 +779,10 @@
         <v>13</v>
       </c>
       <c r="D4">
-        <v>313</v>
+        <v>594</v>
       </c>
       <c r="E4">
-        <v>4.764804384228954</v>
+        <v>3.574222275708526</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -782,10 +796,10 @@
         <v>14</v>
       </c>
       <c r="D5">
-        <v>252</v>
+        <v>478</v>
       </c>
       <c r="E5">
-        <v>3.836200334906378</v>
+        <v>2.876226006378242</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -799,10 +813,10 @@
         <v>13</v>
       </c>
       <c r="D6">
-        <v>1921</v>
+        <v>6263</v>
       </c>
       <c r="E6">
-        <v>29.24341604506013</v>
+        <v>37.685781334617</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -816,10 +830,10 @@
         <v>14</v>
       </c>
       <c r="D7">
-        <v>695</v>
+        <v>1916</v>
       </c>
       <c r="E7">
-        <v>10.57999695539656</v>
+        <v>11.52897286238642</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -833,10 +847,10 @@
         <v>13</v>
       </c>
       <c r="D8">
-        <v>1585</v>
+        <v>2775</v>
       </c>
       <c r="E8">
-        <v>24.12848226518496</v>
+        <v>16.69775558096155</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -850,10 +864,10 @@
         <v>14</v>
       </c>
       <c r="D9">
-        <v>1186</v>
+        <v>2214</v>
       </c>
       <c r="E9">
-        <v>18.05449840158319</v>
+        <v>13.32210120945905</v>
       </c>
     </row>
   </sheetData>
@@ -863,7 +877,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F65"/>
+  <dimension ref="A1:F70"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -903,10 +917,10 @@
         <v>13</v>
       </c>
       <c r="E2">
-        <v>39</v>
+        <v>304</v>
       </c>
       <c r="F2">
-        <v>0.5936976708783681</v>
+        <v>1.829231602382815</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -923,10 +937,10 @@
         <v>14</v>
       </c>
       <c r="E3">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="F3">
-        <v>0.07611508601004718</v>
+        <v>0.1564474396774776</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -943,10 +957,10 @@
         <v>13</v>
       </c>
       <c r="E4">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="F4">
-        <v>0.1978992236261227</v>
+        <v>0.1504302304591131</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -963,10 +977,10 @@
         <v>14</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F5">
-        <v>0.01522301720200944</v>
+        <v>0.01805162765509357</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -983,10 +997,10 @@
         <v>13</v>
       </c>
       <c r="E6">
-        <v>149</v>
+        <v>1215</v>
       </c>
       <c r="F6">
-        <v>2.268229563099406</v>
+        <v>7.310909200312894</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1003,10 +1017,10 @@
         <v>14</v>
       </c>
       <c r="E7">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="F7">
-        <v>0.1674531892221038</v>
+        <v>0.3971358084120585</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1023,10 +1037,10 @@
         <v>13</v>
       </c>
       <c r="E8">
-        <v>65</v>
+        <v>152</v>
       </c>
       <c r="F8">
-        <v>0.9894961181306134</v>
+        <v>0.9146158011914074</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1043,10 +1057,10 @@
         <v>14</v>
       </c>
       <c r="E9">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="F9">
-        <v>0.2131222408281321</v>
+        <v>0.1564474396774776</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1063,10 +1077,10 @@
         <v>13</v>
       </c>
       <c r="E10">
-        <v>41</v>
+        <v>336</v>
       </c>
       <c r="F10">
-        <v>0.6241437052823869</v>
+        <v>2.02178229737048</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1077,16 +1091,16 @@
         <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E11">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F11">
-        <v>0.2740143096361699</v>
+        <v>0.09627534749383236</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1100,13 +1114,13 @@
         <v>14</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E12">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="F12">
-        <v>0.1217841376160755</v>
+        <v>0.1985679042060292</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1114,19 +1128,19 @@
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E13">
-        <v>191</v>
+        <v>10</v>
       </c>
       <c r="F13">
-        <v>2.907596285583803</v>
+        <v>0.06017209218364523</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1140,13 +1154,13 @@
         <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E14">
-        <v>24</v>
+        <v>862</v>
       </c>
       <c r="F14">
-        <v>0.3653524128482265</v>
+        <v>5.186834346230219</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1157,16 +1171,16 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E15">
-        <v>143</v>
+        <v>111</v>
       </c>
       <c r="F15">
-        <v>2.176891459887349</v>
+        <v>0.6679102232384621</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1180,33 +1194,33 @@
         <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E16">
-        <v>55</v>
+        <v>227</v>
       </c>
       <c r="F16">
-        <v>0.8372659461105192</v>
+        <v>1.365906492568747</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E17">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="F17">
-        <v>1.111280255746689</v>
+        <v>0.5054455743426199</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1220,13 +1234,13 @@
         <v>13</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E18">
-        <v>14</v>
+        <v>372</v>
       </c>
       <c r="F18">
-        <v>0.2131222408281321</v>
+        <v>2.238401829231603</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1237,16 +1251,16 @@
         <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E19">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="F19">
-        <v>0.7915968945044908</v>
+        <v>0.2467055779529454</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1260,13 +1274,13 @@
         <v>14</v>
       </c>
       <c r="D20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E20">
-        <v>22</v>
+        <v>90</v>
       </c>
       <c r="F20">
-        <v>0.3349063784442077</v>
+        <v>0.541548829652807</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1274,19 +1288,19 @@
         <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E21">
-        <v>298</v>
+        <v>41</v>
       </c>
       <c r="F21">
-        <v>4.536459126198813</v>
+        <v>0.2467055779529454</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1300,13 +1314,13 @@
         <v>13</v>
       </c>
       <c r="D22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E22">
-        <v>86</v>
+        <v>1039</v>
       </c>
       <c r="F22">
-        <v>1.309179479372812</v>
+        <v>6.251880377880739</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1317,16 +1331,16 @@
         <v>14</v>
       </c>
       <c r="C23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D23" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E23">
-        <v>198</v>
+        <v>288</v>
       </c>
       <c r="F23">
-        <v>3.014157405997869</v>
+        <v>1.732956254888983</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1340,33 +1354,33 @@
         <v>14</v>
       </c>
       <c r="D24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E24">
-        <v>99</v>
+        <v>341</v>
       </c>
       <c r="F24">
-        <v>1.507078702998934</v>
+        <v>2.051868343462302</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C25" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D25" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E25">
-        <v>98</v>
+        <v>200</v>
       </c>
       <c r="F25">
-        <v>1.491855685796925</v>
+        <v>1.203441843672904</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1380,13 +1394,13 @@
         <v>13</v>
       </c>
       <c r="D26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E26">
-        <v>28</v>
+        <v>440</v>
       </c>
       <c r="F26">
-        <v>0.4262444816562643</v>
+        <v>2.64757205608039</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1397,16 +1411,16 @@
         <v>13</v>
       </c>
       <c r="C27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D27" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E27">
-        <v>60</v>
+        <v>111</v>
       </c>
       <c r="F27">
-        <v>0.9133810321205663</v>
+        <v>0.6679102232384621</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1420,13 +1434,13 @@
         <v>14</v>
       </c>
       <c r="D28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E28">
-        <v>57</v>
+        <v>122</v>
       </c>
       <c r="F28">
-        <v>0.867711980514538</v>
+        <v>0.7340995246404717</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1434,19 +1448,19 @@
         <v>7</v>
       </c>
       <c r="B29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C29" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D29" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E29">
-        <v>365</v>
+        <v>99</v>
       </c>
       <c r="F29">
-        <v>5.556401278733445</v>
+        <v>0.5957037126180877</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1460,13 +1474,13 @@
         <v>13</v>
       </c>
       <c r="D30" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E30">
-        <v>165</v>
+        <v>1150</v>
       </c>
       <c r="F30">
-        <v>2.511797838331557</v>
+        <v>6.919790601119201</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1477,16 +1491,16 @@
         <v>14</v>
       </c>
       <c r="C31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D31" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E31">
-        <v>313</v>
+        <v>513</v>
       </c>
       <c r="F31">
-        <v>4.764804384228954</v>
+        <v>3.086828329021</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1500,33 +1514,33 @@
         <v>14</v>
       </c>
       <c r="D32" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E32">
-        <v>277</v>
+        <v>544</v>
       </c>
       <c r="F32">
-        <v>4.216775764956615</v>
+        <v>3.2733618147903</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B33" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C33" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D33" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E33">
-        <v>126</v>
+        <v>547</v>
       </c>
       <c r="F33">
-        <v>1.918100167453189</v>
+        <v>3.291413442445394</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1540,13 +1554,13 @@
         <v>13</v>
       </c>
       <c r="D34" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E34">
-        <v>57</v>
+        <v>326</v>
       </c>
       <c r="F34">
-        <v>0.867711980514538</v>
+        <v>1.961610205186834</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1557,16 +1571,16 @@
         <v>13</v>
       </c>
       <c r="C35" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D35" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E35">
-        <v>79</v>
+        <v>128</v>
       </c>
       <c r="F35">
-        <v>1.202618358958746</v>
+        <v>0.7702027799506589</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1580,13 +1594,13 @@
         <v>14</v>
       </c>
       <c r="D36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E36">
-        <v>81</v>
+        <v>159</v>
       </c>
       <c r="F36">
-        <v>1.233064393362765</v>
+        <v>0.9567362657199591</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1594,19 +1608,19 @@
         <v>8</v>
       </c>
       <c r="B37" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C37" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D37" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E37">
-        <v>452</v>
+        <v>148</v>
       </c>
       <c r="F37">
-        <v>6.880803775308266</v>
+        <v>0.8905469643179493</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1620,13 +1634,13 @@
         <v>13</v>
       </c>
       <c r="D38" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E38">
-        <v>234</v>
+        <v>977</v>
       </c>
       <c r="F38">
-        <v>3.562186025270209</v>
+        <v>5.878813406342139</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1637,16 +1651,16 @@
         <v>14</v>
       </c>
       <c r="C39" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D39" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E39">
-        <v>419</v>
+        <v>549</v>
       </c>
       <c r="F39">
-        <v>6.378444207641955</v>
+        <v>3.303447860882123</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1660,33 +1674,33 @@
         <v>14</v>
       </c>
       <c r="D40" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E40">
-        <v>427</v>
+        <v>734</v>
       </c>
       <c r="F40">
-        <v>6.50022834525803</v>
+        <v>4.416631566279559</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B41" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C41" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D41" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E41">
-        <v>74</v>
+        <v>758</v>
       </c>
       <c r="F41">
-        <v>1.126503272948698</v>
+        <v>4.561044587520309</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1700,13 +1714,13 @@
         <v>13</v>
       </c>
       <c r="D42" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E42">
-        <v>36</v>
+        <v>151</v>
       </c>
       <c r="F42">
-        <v>0.5480286192723398</v>
+        <v>0.9085985919730428</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1717,16 +1731,16 @@
         <v>13</v>
       </c>
       <c r="C43" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D43" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E43">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="F43">
-        <v>0.9894961181306134</v>
+        <v>0.4633251098140683</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1740,13 +1754,13 @@
         <v>14</v>
       </c>
       <c r="D44" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E44">
-        <v>67</v>
+        <v>128</v>
       </c>
       <c r="F44">
-        <v>1.019942152534632</v>
+        <v>0.7702027799506589</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1754,19 +1768,19 @@
         <v>9</v>
       </c>
       <c r="B45" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C45" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D45" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E45">
-        <v>368</v>
+        <v>137</v>
       </c>
       <c r="F45">
-        <v>5.602070330339473</v>
+        <v>0.8243576629159396</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1780,13 +1794,13 @@
         <v>13</v>
       </c>
       <c r="D46" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E46">
-        <v>149</v>
+        <v>663</v>
       </c>
       <c r="F46">
-        <v>2.268229563099406</v>
+        <v>3.989409711775679</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1797,16 +1811,16 @@
         <v>14</v>
       </c>
       <c r="C47" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D47" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E47">
-        <v>369</v>
+        <v>319</v>
       </c>
       <c r="F47">
-        <v>5.617293347541483</v>
+        <v>1.919489740658282</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1820,33 +1834,33 @@
         <v>14</v>
       </c>
       <c r="D48" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E48">
-        <v>272</v>
+        <v>629</v>
       </c>
       <c r="F48">
-        <v>4.140660678946567</v>
+        <v>3.784824598351285</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B49" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C49" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D49" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E49">
-        <v>17</v>
+        <v>495</v>
       </c>
       <c r="F49">
-        <v>0.2587912924341604</v>
+        <v>2.978518563090438</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1860,13 +1874,13 @@
         <v>13</v>
       </c>
       <c r="D50" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E50">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="F50">
-        <v>0.1065611204140661</v>
+        <v>0.1744990673325711</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1877,16 +1891,16 @@
         <v>13</v>
       </c>
       <c r="C51" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D51" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E51">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F51">
-        <v>0.380575430050236</v>
+        <v>0.07220651062037427</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -1900,13 +1914,13 @@
         <v>14</v>
       </c>
       <c r="D52" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E52">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="F52">
-        <v>0.243568275232151</v>
+        <v>0.2045851134243938</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -1914,19 +1928,19 @@
         <v>10</v>
       </c>
       <c r="B53" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C53" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D53" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E53">
-        <v>89</v>
+        <v>40</v>
       </c>
       <c r="F53">
-        <v>1.35484853097884</v>
+        <v>0.2406883687345809</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -1940,13 +1954,13 @@
         <v>13</v>
       </c>
       <c r="D54" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E54">
-        <v>24</v>
+        <v>150</v>
       </c>
       <c r="F54">
-        <v>0.3653524128482265</v>
+        <v>0.9025813827546784</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -1957,16 +1971,16 @@
         <v>14</v>
       </c>
       <c r="C55" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D55" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E55">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="F55">
-        <v>1.111280255746689</v>
+        <v>0.3429809254467778</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -1980,33 +1994,33 @@
         <v>14</v>
       </c>
       <c r="D56" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E56">
-        <v>40</v>
+        <v>134</v>
       </c>
       <c r="F56">
-        <v>0.6089206880803775</v>
+        <v>0.806306035260846</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B57" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C57" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D57" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E57">
-        <v>1</v>
+        <v>96</v>
       </c>
       <c r="F57">
-        <v>0.01522301720200944</v>
+        <v>0.5776520849629941</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -2020,13 +2034,13 @@
         <v>13</v>
       </c>
       <c r="D58" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E58">
         <v>1</v>
       </c>
       <c r="F58">
-        <v>0.01522301720200944</v>
+        <v>0.006017209218364523</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -2037,16 +2051,16 @@
         <v>13</v>
       </c>
       <c r="C59" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D59" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E59">
         <v>1</v>
       </c>
       <c r="F59">
-        <v>0.01522301720200944</v>
+        <v>0.006017209218364523</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -2054,19 +2068,19 @@
         <v>11</v>
       </c>
       <c r="B60" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C60" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D60" t="s">
         <v>13</v>
       </c>
       <c r="E60">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F60">
-        <v>0.06089206880803775</v>
+        <v>0.01203441843672905</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -2077,16 +2091,16 @@
         <v>14</v>
       </c>
       <c r="C61" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D61" t="s">
         <v>13</v>
       </c>
       <c r="E61">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F61">
-        <v>0.04566905160602831</v>
+        <v>0.0541548829652807</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -2097,7 +2111,7 @@
         <v>14</v>
       </c>
       <c r="C62" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D62" t="s">
         <v>14</v>
@@ -2106,18 +2120,18 @@
         <v>2</v>
       </c>
       <c r="F62">
-        <v>0.03044603440401887</v>
+        <v>0.01203441843672905</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B63" t="s">
         <v>14</v>
       </c>
       <c r="C63" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D63" t="s">
         <v>13</v>
@@ -2126,27 +2140,27 @@
         <v>5</v>
       </c>
       <c r="F63">
-        <v>0.07611508601004718</v>
+        <v>0.03008604609182261</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B64" t="s">
         <v>14</v>
       </c>
       <c r="C64" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D64" t="s">
         <v>14</v>
       </c>
       <c r="E64">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F64">
-        <v>0.03044603440401887</v>
+        <v>0.03610325531018713</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -2154,19 +2168,119 @@
         <v>12</v>
       </c>
       <c r="B65" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C65" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D65" t="s">
         <v>13</v>
       </c>
       <c r="E65">
+        <v>8</v>
+      </c>
+      <c r="F65">
+        <v>0.04813767374691618</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" t="s">
+        <v>12</v>
+      </c>
+      <c r="B66" t="s">
+        <v>13</v>
+      </c>
+      <c r="C66" t="s">
+        <v>14</v>
+      </c>
+      <c r="D66" t="s">
+        <v>13</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
+      <c r="F66">
+        <v>0.006017209218364523</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" t="s">
+        <v>12</v>
+      </c>
+      <c r="B67" t="s">
+        <v>14</v>
+      </c>
+      <c r="C67" t="s">
+        <v>13</v>
+      </c>
+      <c r="D67" t="s">
+        <v>13</v>
+      </c>
+      <c r="E67">
+        <v>198</v>
+      </c>
+      <c r="F67">
+        <v>1.191407425236175</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" t="s">
+        <v>12</v>
+      </c>
+      <c r="B68" t="s">
+        <v>14</v>
+      </c>
+      <c r="C68" t="s">
+        <v>13</v>
+      </c>
+      <c r="D68" t="s">
+        <v>14</v>
+      </c>
+      <c r="E68">
+        <v>11</v>
+      </c>
+      <c r="F68">
+        <v>0.06618930140200975</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" t="s">
+        <v>12</v>
+      </c>
+      <c r="B69" t="s">
+        <v>14</v>
+      </c>
+      <c r="C69" t="s">
+        <v>14</v>
+      </c>
+      <c r="D69" t="s">
+        <v>13</v>
+      </c>
+      <c r="E69">
+        <v>9</v>
+      </c>
+      <c r="F69">
+        <v>0.0541548829652807</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" t="s">
+        <v>12</v>
+      </c>
+      <c r="B70" t="s">
+        <v>14</v>
+      </c>
+      <c r="C70" t="s">
+        <v>14</v>
+      </c>
+      <c r="D70" t="s">
+        <v>14</v>
+      </c>
+      <c r="E70">
         <v>2</v>
       </c>
-      <c r="F65">
-        <v>0.03044603440401887</v>
+      <c r="F70">
+        <v>0.01203441843672905</v>
       </c>
     </row>
   </sheetData>
@@ -2204,10 +2318,10 @@
         <v>13</v>
       </c>
       <c r="C2">
-        <v>204</v>
+        <v>1611</v>
       </c>
       <c r="D2">
-        <v>3.105495509209925</v>
+        <v>9.693724050785246</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2218,10 +2332,10 @@
         <v>14</v>
       </c>
       <c r="C3">
-        <v>93</v>
+        <v>206</v>
       </c>
       <c r="D3">
-        <v>1.415740599786878</v>
+        <v>1.239545098983092</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2232,10 +2346,10 @@
         <v>13</v>
       </c>
       <c r="C4">
-        <v>256</v>
+        <v>1325</v>
       </c>
       <c r="D4">
-        <v>3.897092403714416</v>
+        <v>7.972802214332993</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2246,10 +2360,10 @@
         <v>14</v>
       </c>
       <c r="C5">
-        <v>224</v>
+        <v>354</v>
       </c>
       <c r="D5">
-        <v>3.409955853250114</v>
+        <v>2.130092063301041</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2260,10 +2374,10 @@
         <v>13</v>
       </c>
       <c r="C6">
-        <v>471</v>
+        <v>1740</v>
       </c>
       <c r="D6">
-        <v>7.170041102146446</v>
+        <v>10.46994403995427</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -2274,10 +2388,10 @@
         <v>14</v>
       </c>
       <c r="C7">
-        <v>371</v>
+        <v>672</v>
       </c>
       <c r="D7">
-        <v>5.647739381945502</v>
+        <v>4.04356459474096</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -2288,10 +2402,10 @@
         <v>13</v>
       </c>
       <c r="C8">
-        <v>656</v>
+        <v>2214</v>
       </c>
       <c r="D8">
-        <v>9.986299284518191</v>
+        <v>13.32210120945905</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -2302,10 +2416,10 @@
         <v>14</v>
       </c>
       <c r="C9">
-        <v>707</v>
+        <v>1312</v>
       </c>
       <c r="D9">
-        <v>10.76267316182067</v>
+        <v>7.894578494494253</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -2316,10 +2430,10 @@
         <v>13</v>
       </c>
       <c r="C10">
-        <v>869</v>
+        <v>1980</v>
       </c>
       <c r="D10">
-        <v>13.2288019485462</v>
+        <v>11.91407425236175</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -2330,10 +2444,10 @@
         <v>14</v>
       </c>
       <c r="C11">
-        <v>1006</v>
+        <v>1799</v>
       </c>
       <c r="D11">
-        <v>15.31435530522149</v>
+        <v>10.82495938383778</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -2344,10 +2458,10 @@
         <v>13</v>
       </c>
       <c r="C12">
-        <v>627</v>
+        <v>1210</v>
       </c>
       <c r="D12">
-        <v>9.544831785659918</v>
+        <v>7.280823154221072</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -2358,10 +2472,10 @@
         <v>14</v>
       </c>
       <c r="C13">
-        <v>773</v>
+        <v>1389</v>
       </c>
       <c r="D13">
-        <v>11.76739229715329</v>
+        <v>8.357903604308321</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -2372,10 +2486,10 @@
         <v>13</v>
       </c>
       <c r="C14">
-        <v>137</v>
+        <v>248</v>
       </c>
       <c r="D14">
-        <v>2.085553356675293</v>
+        <v>1.492267886154402</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -2386,10 +2500,10 @@
         <v>14</v>
       </c>
       <c r="C15">
-        <v>154</v>
+        <v>304</v>
       </c>
       <c r="D15">
-        <v>2.344344649109454</v>
+        <v>1.829231602382815</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -2400,10 +2514,10 @@
         <v>13</v>
       </c>
       <c r="C16">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D16">
-        <v>0.09133810321205663</v>
+        <v>0.0782237198387388</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -2414,10 +2528,10 @@
         <v>14</v>
       </c>
       <c r="C17">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D17">
-        <v>0.09133810321205663</v>
+        <v>0.0782237198387388</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -2428,10 +2542,10 @@
         <v>13</v>
       </c>
       <c r="C18">
-        <v>7</v>
+        <v>217</v>
       </c>
       <c r="D18">
-        <v>0.1065611204140661</v>
+        <v>1.305734400385101</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -2442,10 +2556,10 @@
         <v>14</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D19">
-        <v>0.03044603440401887</v>
+        <v>0.07220651062037427</v>
       </c>
     </row>
   </sheetData>
@@ -2483,10 +2597,10 @@
         <v>13</v>
       </c>
       <c r="C2">
-        <v>266</v>
+        <v>1696</v>
       </c>
       <c r="D2">
-        <v>4.049322575734511</v>
+        <v>10.20518683434623</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2497,10 +2611,10 @@
         <v>14</v>
       </c>
       <c r="C3">
-        <v>31</v>
+        <v>121</v>
       </c>
       <c r="D3">
-        <v>0.4719135332622926</v>
+        <v>0.7280823154221072</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2511,10 +2625,10 @@
         <v>13</v>
       </c>
       <c r="C4">
-        <v>393</v>
+        <v>1458</v>
       </c>
       <c r="D4">
-        <v>5.982645760389709</v>
+        <v>8.773091040375473</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2525,10 +2639,10 @@
         <v>14</v>
       </c>
       <c r="C5">
-        <v>87</v>
+        <v>221</v>
       </c>
       <c r="D5">
-        <v>1.324402496574821</v>
+        <v>1.32980323725856</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2539,10 +2653,10 @@
         <v>13</v>
       </c>
       <c r="C6">
-        <v>621</v>
+        <v>1842</v>
       </c>
       <c r="D6">
-        <v>9.453493682447862</v>
+        <v>11.08369938022745</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -2553,10 +2667,10 @@
         <v>14</v>
       </c>
       <c r="C7">
-        <v>221</v>
+        <v>570</v>
       </c>
       <c r="D7">
-        <v>3.364286801644086</v>
+        <v>3.429809254467778</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -2567,10 +2681,10 @@
         <v>13</v>
       </c>
       <c r="C8">
-        <v>836</v>
+        <v>2256</v>
       </c>
       <c r="D8">
-        <v>12.72644238087989</v>
+        <v>13.57482399663036</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -2581,10 +2695,10 @@
         <v>14</v>
       </c>
       <c r="C9">
-        <v>527</v>
+        <v>1270</v>
       </c>
       <c r="D9">
-        <v>8.022530065458975</v>
+        <v>7.641855707322944</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -2595,10 +2709,10 @@
         <v>13</v>
       </c>
       <c r="C10">
-        <v>1076</v>
+        <v>2196</v>
       </c>
       <c r="D10">
-        <v>16.37996650936216</v>
+        <v>13.21379144352849</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -2609,10 +2723,10 @@
         <v>14</v>
       </c>
       <c r="C11">
-        <v>799</v>
+        <v>1583</v>
       </c>
       <c r="D11">
-        <v>12.16319074440554</v>
+        <v>9.525242192671039</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -2623,10 +2737,10 @@
         <v>13</v>
       </c>
       <c r="C12">
-        <v>876</v>
+        <v>1571</v>
       </c>
       <c r="D12">
-        <v>13.33536306896027</v>
+        <v>9.453035682050665</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -2637,10 +2751,10 @@
         <v>14</v>
       </c>
       <c r="C13">
-        <v>524</v>
+        <v>1028</v>
       </c>
       <c r="D13">
-        <v>7.976861013852946</v>
+        <v>6.185691076478729</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -2651,10 +2765,10 @@
         <v>13</v>
       </c>
       <c r="C14">
-        <v>204</v>
+        <v>347</v>
       </c>
       <c r="D14">
-        <v>3.105495509209925</v>
+        <v>2.087971598772489</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -2665,10 +2779,10 @@
         <v>14</v>
       </c>
       <c r="C15">
-        <v>87</v>
+        <v>205</v>
       </c>
       <c r="D15">
-        <v>1.324402496574821</v>
+        <v>1.233527889764727</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -2679,10 +2793,10 @@
         <v>13</v>
       </c>
       <c r="C16">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D16">
-        <v>0.137007154818085</v>
+        <v>0.1022925567121969</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -2693,10 +2807,10 @@
         <v>14</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D17">
-        <v>0.04566905160602831</v>
+        <v>0.0541548829652807</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -2707,10 +2821,10 @@
         <v>13</v>
       </c>
       <c r="C18">
-        <v>7</v>
+        <v>216</v>
       </c>
       <c r="D18">
-        <v>0.1065611204140661</v>
+        <v>1.299717191166737</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -2721,10 +2835,10 @@
         <v>14</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D19">
-        <v>0.03044603440401887</v>
+        <v>0.0782237198387388</v>
       </c>
     </row>
   </sheetData>
@@ -2762,10 +2876,10 @@
         <v>13</v>
       </c>
       <c r="C2">
-        <v>617</v>
+        <v>2379</v>
       </c>
       <c r="D2">
-        <v>9.392601613639824</v>
+        <v>14.3149407304892</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2776,10 +2890,10 @@
         <v>14</v>
       </c>
       <c r="C3">
-        <v>565</v>
+        <v>1072</v>
       </c>
       <c r="D3">
-        <v>8.601004719135332</v>
+        <v>6.450448282086768</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2790,10 +2904,10 @@
         <v>13</v>
       </c>
       <c r="C4">
-        <v>2616</v>
+        <v>8179</v>
       </c>
       <c r="D4">
-        <v>39.82341300045669</v>
+        <v>49.21475419700343</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2804,10 +2918,10 @@
         <v>14</v>
       </c>
       <c r="C5">
-        <v>2771</v>
+        <v>4989</v>
       </c>
       <c r="D5">
-        <v>42.18298066676815</v>
+        <v>30.0198567904206</v>
       </c>
     </row>
   </sheetData>
@@ -2845,10 +2959,10 @@
         <v>13</v>
       </c>
       <c r="C2">
-        <v>782</v>
+        <v>2561</v>
       </c>
       <c r="D2">
-        <v>11.90439945197138</v>
+        <v>15.41007280823154</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2859,10 +2973,10 @@
         <v>14</v>
       </c>
       <c r="C3">
-        <v>400</v>
+        <v>890</v>
       </c>
       <c r="D3">
-        <v>6.089206880803776</v>
+        <v>5.355316204344425</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2873,10 +2987,10 @@
         <v>13</v>
       </c>
       <c r="C4">
-        <v>3506</v>
+        <v>9038</v>
       </c>
       <c r="D4">
-        <v>53.37189831024509</v>
+        <v>54.38353691557856</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2887,10 +3001,10 @@
         <v>14</v>
       </c>
       <c r="C5">
-        <v>1881</v>
+        <v>4130</v>
       </c>
       <c r="D5">
-        <v>28.63449535697976</v>
+        <v>24.85107407184548</v>
       </c>
     </row>
   </sheetData>
@@ -2928,10 +3042,10 @@
         <v>13</v>
       </c>
       <c r="C2">
-        <v>2390</v>
+        <v>8230</v>
       </c>
       <c r="D2">
-        <v>36.38301111280256</v>
+        <v>49.52163186714002</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2942,10 +3056,10 @@
         <v>14</v>
       </c>
       <c r="C3">
-        <v>843</v>
+        <v>2328</v>
       </c>
       <c r="D3">
-        <v>12.83300350129396</v>
+        <v>14.00806306035261</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2956,10 +3070,10 @@
         <v>13</v>
       </c>
       <c r="C4">
-        <v>1898</v>
+        <v>3369</v>
       </c>
       <c r="D4">
-        <v>28.89328664941391</v>
+        <v>20.27197785667008</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2970,10 +3084,10 @@
         <v>14</v>
       </c>
       <c r="C5">
-        <v>1438</v>
+        <v>2692</v>
       </c>
       <c r="D5">
-        <v>21.89069873648957</v>
+        <v>16.1983272158373</v>
       </c>
     </row>
   </sheetData>
@@ -2983,7 +3097,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3017,10 +3131,10 @@
         <v>13</v>
       </c>
       <c r="D2">
-        <v>44</v>
+        <v>330</v>
       </c>
       <c r="E2">
-        <v>0.6698127568884154</v>
+        <v>1.985679042060292</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -3034,10 +3148,10 @@
         <v>14</v>
       </c>
       <c r="D3">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="E3">
-        <v>0.2131222408281321</v>
+        <v>0.1684818581142066</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -3051,10 +3165,10 @@
         <v>13</v>
       </c>
       <c r="D4">
-        <v>160</v>
+        <v>1281</v>
       </c>
       <c r="E4">
-        <v>2.43568275232151</v>
+        <v>7.708045008724953</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -3068,10 +3182,10 @@
         <v>14</v>
       </c>
       <c r="D5">
-        <v>79</v>
+        <v>178</v>
       </c>
       <c r="E5">
-        <v>1.202618358958746</v>
+        <v>1.071063240868885</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -3085,10 +3199,10 @@
         <v>13</v>
       </c>
       <c r="D6">
-        <v>41</v>
+        <v>352</v>
       </c>
       <c r="E6">
-        <v>0.6241437052823869</v>
+        <v>2.118057644864312</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -3102,10 +3216,10 @@
         <v>14</v>
       </c>
       <c r="D7">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="E7">
-        <v>0.3957984472522454</v>
+        <v>0.2587399963896745</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -3119,10 +3233,10 @@
         <v>13</v>
       </c>
       <c r="D8">
-        <v>215</v>
+        <v>973</v>
       </c>
       <c r="E8">
-        <v>3.27294869843203</v>
+        <v>5.85474456946868</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -3136,10 +3250,10 @@
         <v>14</v>
       </c>
       <c r="D9">
-        <v>198</v>
+        <v>311</v>
       </c>
       <c r="E9">
-        <v>3.014157405997869</v>
+        <v>1.871352066911367</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -3153,10 +3267,10 @@
         <v>13</v>
       </c>
       <c r="D10">
-        <v>87</v>
+        <v>413</v>
       </c>
       <c r="E10">
-        <v>1.324402496574821</v>
+        <v>2.485107407184548</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -3170,10 +3284,10 @@
         <v>14</v>
       </c>
       <c r="D11">
-        <v>74</v>
+        <v>131</v>
       </c>
       <c r="E11">
-        <v>1.126503272948698</v>
+        <v>0.7882544076057525</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -3187,10 +3301,10 @@
         <v>13</v>
       </c>
       <c r="D12">
-        <v>384</v>
+        <v>1327</v>
       </c>
       <c r="E12">
-        <v>5.845638605571624</v>
+        <v>7.984836632769722</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -3204,10 +3318,10 @@
         <v>14</v>
       </c>
       <c r="D13">
-        <v>297</v>
+        <v>541</v>
       </c>
       <c r="E13">
-        <v>4.521236108996804</v>
+        <v>3.255310187135207</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -3221,10 +3335,10 @@
         <v>13</v>
       </c>
       <c r="D14">
-        <v>126</v>
+        <v>551</v>
       </c>
       <c r="E14">
-        <v>1.918100167453189</v>
+        <v>3.315482279318852</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -3238,10 +3352,10 @@
         <v>14</v>
       </c>
       <c r="D15">
-        <v>117</v>
+        <v>221</v>
       </c>
       <c r="E15">
-        <v>1.781093012635104</v>
+        <v>1.32980323725856</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -3255,10 +3369,10 @@
         <v>13</v>
       </c>
       <c r="D16">
-        <v>530</v>
+        <v>1663</v>
       </c>
       <c r="E16">
-        <v>8.068199117065001</v>
+        <v>10.0066189301402</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -3272,10 +3386,10 @@
         <v>14</v>
       </c>
       <c r="D17">
-        <v>590</v>
+        <v>1091</v>
       </c>
       <c r="E17">
-        <v>8.981580149185568</v>
+        <v>6.564775257235694</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -3289,10 +3403,10 @@
         <v>13</v>
       </c>
       <c r="D18">
-        <v>183</v>
+        <v>454</v>
       </c>
       <c r="E18">
-        <v>2.785812147967727</v>
+        <v>2.731812985137493</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -3306,10 +3420,10 @@
         <v>14</v>
       </c>
       <c r="D19">
-        <v>160</v>
+        <v>307</v>
       </c>
       <c r="E19">
-        <v>2.43568275232151</v>
+        <v>1.847283230037909</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -3323,10 +3437,10 @@
         <v>13</v>
       </c>
       <c r="D20">
-        <v>686</v>
+        <v>1526</v>
       </c>
       <c r="E20">
-        <v>10.44298980057847</v>
+        <v>9.182261267224263</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -3340,10 +3454,10 @@
         <v>14</v>
       </c>
       <c r="D21">
-        <v>846</v>
+        <v>1492</v>
       </c>
       <c r="E21">
-        <v>12.87867255289998</v>
+        <v>8.977676153799868</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -3357,10 +3471,10 @@
         <v>13</v>
       </c>
       <c r="D22">
-        <v>110</v>
+        <v>228</v>
       </c>
       <c r="E22">
-        <v>1.674531892221038</v>
+        <v>1.371923701787111</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -3374,10 +3488,10 @@
         <v>14</v>
       </c>
       <c r="D23">
-        <v>132</v>
+        <v>265</v>
       </c>
       <c r="E23">
-        <v>2.009438270665246</v>
+        <v>1.594560442866598</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -3391,10 +3505,10 @@
         <v>13</v>
       </c>
       <c r="D24">
-        <v>517</v>
+        <v>982</v>
       </c>
       <c r="E24">
-        <v>7.870299893438879</v>
+        <v>5.908899452433961</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -3408,10 +3522,10 @@
         <v>14</v>
       </c>
       <c r="D25">
-        <v>641</v>
+        <v>1124</v>
       </c>
       <c r="E25">
-        <v>9.757954026488051</v>
+        <v>6.763343161441723</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -3425,10 +3539,10 @@
         <v>13</v>
       </c>
       <c r="D26">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="E26">
-        <v>0.3653524128482265</v>
+        <v>0.2467055779529454</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -3442,10 +3556,10 @@
         <v>14</v>
       </c>
       <c r="D27">
-        <v>41</v>
+        <v>74</v>
       </c>
       <c r="E27">
-        <v>0.6241437052823869</v>
+        <v>0.4452734821589747</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -3459,10 +3573,10 @@
         <v>13</v>
       </c>
       <c r="D28">
-        <v>113</v>
+        <v>207</v>
       </c>
       <c r="E28">
-        <v>1.720200943827066</v>
+        <v>1.245562308201456</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -3476,10 +3590,10 @@
         <v>14</v>
       </c>
       <c r="D29">
-        <v>113</v>
+        <v>230</v>
       </c>
       <c r="E29">
-        <v>1.720200943827066</v>
+        <v>1.38395812022384</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -3496,7 +3610,7 @@
         <v>2</v>
       </c>
       <c r="E30">
-        <v>0.03044603440401887</v>
+        <v>0.01203441843672905</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -3510,10 +3624,10 @@
         <v>14</v>
       </c>
       <c r="D31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E31">
-        <v>0.01522301720200944</v>
+        <v>0.01203441843672905</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -3527,10 +3641,10 @@
         <v>13</v>
       </c>
       <c r="D32">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E32">
-        <v>0.06089206880803775</v>
+        <v>0.06618930140200975</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -3544,10 +3658,10 @@
         <v>14</v>
       </c>
       <c r="D33">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E33">
-        <v>0.07611508601004718</v>
+        <v>0.06618930140200975</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -3555,16 +3669,16 @@
         <v>12</v>
       </c>
       <c r="B34" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C34" t="s">
         <v>13</v>
       </c>
       <c r="D34">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E34">
-        <v>0.1065611204140661</v>
+        <v>0.04813767374691618</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -3572,16 +3686,50 @@
         <v>12</v>
       </c>
       <c r="B35" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C35" t="s">
         <v>14</v>
       </c>
       <c r="D35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E35">
-        <v>0.03044603440401887</v>
+        <v>0.006017209218364523</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36">
+        <v>209</v>
+      </c>
+      <c r="E36">
+        <v>1.257596726638185</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37">
+        <v>11</v>
+      </c>
+      <c r="E37">
+        <v>0.06618930140200975</v>
       </c>
     </row>
   </sheetData>
@@ -3590,614 +3738,6 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E35"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2">
-        <v>52</v>
-      </c>
-      <c r="E2">
-        <v>0.7915968945044908</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3">
-        <v>6</v>
-      </c>
-      <c r="E3">
-        <v>0.09133810321205663</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4">
-        <v>214</v>
-      </c>
-      <c r="E4">
-        <v>3.25772568123002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5">
-        <v>25</v>
-      </c>
-      <c r="E5">
-        <v>0.380575430050236</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6">
-        <v>59</v>
-      </c>
-      <c r="E6">
-        <v>0.8981580149185567</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7">
-        <v>8</v>
-      </c>
-      <c r="E7">
-        <v>0.1217841376160755</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8">
-        <v>334</v>
-      </c>
-      <c r="E8">
-        <v>5.084487745471153</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9">
-        <v>79</v>
-      </c>
-      <c r="E9">
-        <v>1.202618358958746</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10">
-        <v>125</v>
-      </c>
-      <c r="E10">
-        <v>1.90287715025118</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11">
-        <v>36</v>
-      </c>
-      <c r="E11">
-        <v>0.5480286192723398</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12">
-        <v>496</v>
-      </c>
-      <c r="E12">
-        <v>7.550616532196681</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13">
-        <v>185</v>
-      </c>
-      <c r="E13">
-        <v>2.816258182371746</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14">
-        <v>158</v>
-      </c>
-      <c r="E14">
-        <v>2.405236717917491</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15">
-        <v>85</v>
-      </c>
-      <c r="E15">
-        <v>1.293956462170802</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16">
-        <v>678</v>
-      </c>
-      <c r="E16">
-        <v>10.3212056629624</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17">
-        <v>442</v>
-      </c>
-      <c r="E17">
-        <v>6.728573603288172</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18">
-        <v>205</v>
-      </c>
-      <c r="E18">
-        <v>3.120718526411935</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19">
-        <v>138</v>
-      </c>
-      <c r="E19">
-        <v>2.100776373877302</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" t="s">
-        <v>13</v>
-      </c>
-      <c r="D20">
-        <v>871</v>
-      </c>
-      <c r="E20">
-        <v>13.25924798295022</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21">
-        <v>661</v>
-      </c>
-      <c r="E21">
-        <v>10.06241437052824</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" t="s">
-        <v>13</v>
-      </c>
-      <c r="D22">
-        <v>139</v>
-      </c>
-      <c r="E22">
-        <v>2.115999391079312</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" t="s">
-        <v>9</v>
-      </c>
-      <c r="B23" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" t="s">
-        <v>14</v>
-      </c>
-      <c r="D23">
-        <v>103</v>
-      </c>
-      <c r="E23">
-        <v>1.567970771806972</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" t="s">
-        <v>9</v>
-      </c>
-      <c r="B24" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" t="s">
-        <v>13</v>
-      </c>
-      <c r="D24">
-        <v>737</v>
-      </c>
-      <c r="E24">
-        <v>11.21936367788096</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" t="s">
-        <v>9</v>
-      </c>
-      <c r="B25" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25" t="s">
-        <v>14</v>
-      </c>
-      <c r="D25">
-        <v>421</v>
-      </c>
-      <c r="E25">
-        <v>6.408890242045974</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" t="s">
-        <v>10</v>
-      </c>
-      <c r="B26" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" t="s">
-        <v>13</v>
-      </c>
-      <c r="D26">
-        <v>42</v>
-      </c>
-      <c r="E26">
-        <v>0.6393667224843964</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" t="s">
-        <v>10</v>
-      </c>
-      <c r="B27" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" t="s">
-        <v>14</v>
-      </c>
-      <c r="D27">
-        <v>23</v>
-      </c>
-      <c r="E27">
-        <v>0.3501293956462171</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" t="s">
-        <v>10</v>
-      </c>
-      <c r="B28" t="s">
-        <v>14</v>
-      </c>
-      <c r="C28" t="s">
-        <v>13</v>
-      </c>
-      <c r="D28">
-        <v>162</v>
-      </c>
-      <c r="E28">
-        <v>2.466128786725529</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" t="s">
-        <v>10</v>
-      </c>
-      <c r="B29" t="s">
-        <v>14</v>
-      </c>
-      <c r="C29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D29">
-        <v>64</v>
-      </c>
-      <c r="E29">
-        <v>0.974273100928604</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" t="s">
-        <v>11</v>
-      </c>
-      <c r="B30" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" t="s">
-        <v>13</v>
-      </c>
-      <c r="D30">
-        <v>2</v>
-      </c>
-      <c r="E30">
-        <v>0.03044603440401887</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" t="s">
-        <v>11</v>
-      </c>
-      <c r="B31" t="s">
-        <v>13</v>
-      </c>
-      <c r="C31" t="s">
-        <v>14</v>
-      </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-      <c r="E31">
-        <v>0.01522301720200944</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" t="s">
-        <v>11</v>
-      </c>
-      <c r="B32" t="s">
-        <v>14</v>
-      </c>
-      <c r="C32" t="s">
-        <v>13</v>
-      </c>
-      <c r="D32">
-        <v>7</v>
-      </c>
-      <c r="E32">
-        <v>0.1065611204140661</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" t="s">
-        <v>11</v>
-      </c>
-      <c r="B33" t="s">
-        <v>14</v>
-      </c>
-      <c r="C33" t="s">
-        <v>14</v>
-      </c>
-      <c r="D33">
-        <v>2</v>
-      </c>
-      <c r="E33">
-        <v>0.03044603440401887</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" t="s">
-        <v>12</v>
-      </c>
-      <c r="B34" t="s">
-        <v>14</v>
-      </c>
-      <c r="C34" t="s">
-        <v>13</v>
-      </c>
-      <c r="D34">
-        <v>7</v>
-      </c>
-      <c r="E34">
-        <v>0.1065611204140661</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" t="s">
-        <v>12</v>
-      </c>
-      <c r="B35" t="s">
-        <v>14</v>
-      </c>
-      <c r="C35" t="s">
-        <v>14</v>
-      </c>
-      <c r="D35">
-        <v>2</v>
-      </c>
-      <c r="E35">
-        <v>0.03044603440401887</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E36"/>
   <sheetViews>
@@ -4210,7 +3750,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>16</v>
@@ -4233,10 +3773,10 @@
         <v>13</v>
       </c>
       <c r="D2">
-        <v>188</v>
+        <v>329</v>
       </c>
       <c r="E2">
-        <v>2.861927233977775</v>
+        <v>1.979661832841928</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -4250,10 +3790,10 @@
         <v>14</v>
       </c>
       <c r="D3">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="E3">
-        <v>0.243568275232151</v>
+        <v>0.1744990673325711</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -4267,10 +3807,10 @@
         <v>13</v>
       </c>
       <c r="D4">
-        <v>78</v>
+        <v>1367</v>
       </c>
       <c r="E4">
-        <v>1.187395341756736</v>
+        <v>8.225525001504302</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -4284,10 +3824,10 @@
         <v>14</v>
       </c>
       <c r="D5">
-        <v>15</v>
+        <v>92</v>
       </c>
       <c r="E5">
-        <v>0.2283452580301416</v>
+        <v>0.5535832480895361</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -4301,10 +3841,10 @@
         <v>13</v>
       </c>
       <c r="D6">
-        <v>232</v>
+        <v>369</v>
       </c>
       <c r="E6">
-        <v>3.53173999086619</v>
+        <v>2.220350201576509</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -4318,10 +3858,10 @@
         <v>14</v>
       </c>
       <c r="D7">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E7">
-        <v>0.3653524128482265</v>
+        <v>0.1564474396774776</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -4335,10 +3875,10 @@
         <v>13</v>
       </c>
       <c r="D8">
-        <v>161</v>
+        <v>1089</v>
       </c>
       <c r="E8">
-        <v>2.45090576952352</v>
+        <v>6.552740838798965</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -4352,10 +3892,10 @@
         <v>14</v>
       </c>
       <c r="D9">
-        <v>63</v>
+        <v>195</v>
       </c>
       <c r="E9">
-        <v>0.9590500837265946</v>
+        <v>1.173355797581082</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -4369,10 +3909,10 @@
         <v>13</v>
       </c>
       <c r="D10">
-        <v>371</v>
+        <v>462</v>
       </c>
       <c r="E10">
-        <v>5.647739381945502</v>
+        <v>2.779950658884409</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -4386,10 +3926,10 @@
         <v>14</v>
       </c>
       <c r="D11">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="E11">
-        <v>1.522301720200944</v>
+        <v>0.4934111559058908</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -4403,10 +3943,10 @@
         <v>13</v>
       </c>
       <c r="D12">
-        <v>250</v>
+        <v>1380</v>
       </c>
       <c r="E12">
-        <v>3.80575430050236</v>
+        <v>8.303748721343041</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -4420,10 +3960,10 @@
         <v>14</v>
       </c>
       <c r="D13">
-        <v>121</v>
+        <v>488</v>
       </c>
       <c r="E13">
-        <v>1.841985081443142</v>
+        <v>2.936398098561887</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -4437,10 +3977,10 @@
         <v>13</v>
       </c>
       <c r="D14">
-        <v>463</v>
+        <v>562</v>
       </c>
       <c r="E14">
-        <v>7.04825696453037</v>
+        <v>3.381671580720861</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -4454,10 +3994,10 @@
         <v>14</v>
       </c>
       <c r="D15">
-        <v>193</v>
+        <v>210</v>
       </c>
       <c r="E15">
-        <v>2.938042319987822</v>
+        <v>1.26361393585655</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -4471,10 +4011,10 @@
         <v>13</v>
       </c>
       <c r="D16">
-        <v>373</v>
+        <v>1694</v>
       </c>
       <c r="E16">
-        <v>5.67818541634952</v>
+        <v>10.1931524159095</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -4488,10 +4028,10 @@
         <v>14</v>
       </c>
       <c r="D17">
-        <v>334</v>
+        <v>1060</v>
       </c>
       <c r="E17">
-        <v>5.084487745471153</v>
+        <v>6.378241771466393</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -4505,10 +4045,10 @@
         <v>13</v>
       </c>
       <c r="D18">
-        <v>578</v>
+        <v>485</v>
       </c>
       <c r="E18">
-        <v>8.798903942761456</v>
+        <v>2.918346470906794</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -4522,10 +4062,10 @@
         <v>14</v>
       </c>
       <c r="D19">
-        <v>291</v>
+        <v>276</v>
       </c>
       <c r="E19">
-        <v>4.429898005784747</v>
+        <v>1.660749744268608</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -4539,10 +4079,10 @@
         <v>13</v>
       </c>
       <c r="D20">
-        <v>498</v>
+        <v>1711</v>
       </c>
       <c r="E20">
-        <v>7.581062566600701</v>
+        <v>10.2954449726217</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -4556,10 +4096,10 @@
         <v>14</v>
       </c>
       <c r="D21">
-        <v>508</v>
+        <v>1307</v>
       </c>
       <c r="E21">
-        <v>7.733292738620795</v>
+        <v>7.864492448402431</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -4573,10 +4113,10 @@
         <v>13</v>
       </c>
       <c r="D22">
-        <v>442</v>
+        <v>279</v>
       </c>
       <c r="E22">
-        <v>6.728573603288172</v>
+        <v>1.678801371923702</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -4590,10 +4130,10 @@
         <v>14</v>
       </c>
       <c r="D23">
-        <v>185</v>
+        <v>214</v>
       </c>
       <c r="E23">
-        <v>2.816258182371746</v>
+        <v>1.287682772730008</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -4607,10 +4147,10 @@
         <v>13</v>
       </c>
       <c r="D24">
-        <v>434</v>
+        <v>1292</v>
       </c>
       <c r="E24">
-        <v>6.606789465672096</v>
+        <v>7.774234310126964</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -4624,10 +4164,10 @@
         <v>14</v>
       </c>
       <c r="D25">
-        <v>339</v>
+        <v>814</v>
       </c>
       <c r="E25">
-        <v>5.160602831481199</v>
+        <v>4.898008303748721</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -4641,10 +4181,10 @@
         <v>13</v>
       </c>
       <c r="D26">
-        <v>106</v>
+        <v>63</v>
       </c>
       <c r="E26">
-        <v>1.613639823413</v>
+        <v>0.3790841807569649</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -4658,10 +4198,10 @@
         <v>14</v>
       </c>
       <c r="D27">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="E27">
-        <v>0.4719135332622926</v>
+        <v>0.3128948793549552</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -4675,10 +4215,10 @@
         <v>13</v>
       </c>
       <c r="D28">
-        <v>98</v>
+        <v>284</v>
       </c>
       <c r="E28">
-        <v>1.491855685796925</v>
+        <v>1.708887418015524</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -4692,10 +4232,10 @@
         <v>14</v>
       </c>
       <c r="D29">
-        <v>56</v>
+        <v>153</v>
       </c>
       <c r="E29">
-        <v>0.8524889633125285</v>
+        <v>0.9206330104097719</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -4709,10 +4249,10 @@
         <v>13</v>
       </c>
       <c r="D30">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E30">
-        <v>0.07611508601004718</v>
+        <v>0.01805162765509357</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -4729,7 +4269,7 @@
         <v>1</v>
       </c>
       <c r="E31">
-        <v>0.01522301720200944</v>
+        <v>0.006017209218364523</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -4743,10 +4283,10 @@
         <v>13</v>
       </c>
       <c r="D32">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="E32">
-        <v>0.06089206880803775</v>
+        <v>0.08424092905710331</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -4760,10 +4300,10 @@
         <v>14</v>
       </c>
       <c r="D33">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E33">
-        <v>0.03044603440401887</v>
+        <v>0.04813767374691618</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -4777,10 +4317,10 @@
         <v>13</v>
       </c>
       <c r="D34">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E34">
-        <v>0.07611508601004718</v>
+        <v>0.0541548829652807</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -4788,16 +4328,16 @@
         <v>12</v>
       </c>
       <c r="B35" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C35" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D35">
-        <v>2</v>
+        <v>207</v>
       </c>
       <c r="E35">
-        <v>0.03044603440401887</v>
+        <v>1.245562308201456</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -4808,13 +4348,655 @@
         <v>14</v>
       </c>
       <c r="C36" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D36">
+        <v>13</v>
+      </c>
+      <c r="E36">
+        <v>0.0782237198387388</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2">
+        <v>1519</v>
+      </c>
+      <c r="E2">
+        <v>9.14014080269571</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3">
+        <v>92</v>
+      </c>
+      <c r="E3">
+        <v>0.5535832480895361</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4">
+        <v>177</v>
+      </c>
+      <c r="E4">
+        <v>1.06504603165052</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5">
+        <v>29</v>
+      </c>
+      <c r="E5">
+        <v>0.1744990673325711</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6">
+        <v>1198</v>
+      </c>
+      <c r="E6">
+        <v>7.208616643600697</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7">
+        <v>127</v>
+      </c>
+      <c r="E7">
+        <v>0.7641855707322943</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8">
+        <v>260</v>
+      </c>
+      <c r="E8">
+        <v>1.564474396774776</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9">
+        <v>94</v>
+      </c>
+      <c r="E9">
+        <v>0.5656176665262651</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10">
+        <v>1411</v>
+      </c>
+      <c r="E10">
+        <v>8.490282207112342</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11">
+        <v>329</v>
+      </c>
+      <c r="E11">
+        <v>1.979661832841928</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12">
+        <v>431</v>
+      </c>
+      <c r="E12">
+        <v>2.593417173115109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13">
+        <v>241</v>
+      </c>
+      <c r="E13">
+        <v>1.45014742162585</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14">
+        <v>1590</v>
+      </c>
+      <c r="E14">
+        <v>9.56736265719959</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15">
+        <v>624</v>
+      </c>
+      <c r="E15">
+        <v>3.754738552259462</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16">
+        <v>666</v>
+      </c>
+      <c r="E16">
+        <v>4.007461339430772</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17">
+        <v>646</v>
+      </c>
+      <c r="E17">
+        <v>3.887117155063482</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18">
+        <v>1303</v>
+      </c>
+      <c r="E18">
+        <v>7.840423611528973</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19">
+        <v>677</v>
+      </c>
+      <c r="E19">
+        <v>4.073650640832781</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20">
+        <v>893</v>
+      </c>
+      <c r="E20">
+        <v>5.373367831999518</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21">
+        <v>906</v>
+      </c>
+      <c r="E21">
+        <v>5.451591551838257</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22">
+        <v>814</v>
+      </c>
+      <c r="E22">
+        <v>4.898008303748721</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23">
+        <v>396</v>
+      </c>
+      <c r="E23">
+        <v>2.382814850472351</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24">
+        <v>757</v>
+      </c>
+      <c r="E24">
+        <v>4.555027378301943</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25">
+        <v>632</v>
+      </c>
+      <c r="E25">
+        <v>3.802876226006378</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26">
+        <v>179</v>
+      </c>
+      <c r="E26">
+        <v>1.07708045008725</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27">
+        <v>69</v>
+      </c>
+      <c r="E27">
+        <v>0.415187436067152</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28">
+        <v>168</v>
+      </c>
+      <c r="E28">
+        <v>1.01089114868524</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29">
+        <v>136</v>
+      </c>
+      <c r="E29">
+        <v>0.818340453697575</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30">
+        <v>10</v>
+      </c>
+      <c r="E30">
+        <v>0.06017209218364523</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31">
+        <v>3</v>
+      </c>
+      <c r="E31">
+        <v>0.01805162765509357</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32">
+        <v>7</v>
+      </c>
+      <c r="E32">
+        <v>0.04212046452855166</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33">
+        <v>6</v>
+      </c>
+      <c r="E33">
+        <v>0.03610325531018713</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34">
+        <v>206</v>
+      </c>
+      <c r="E34">
+        <v>1.239545098983092</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D35">
+        <v>11</v>
+      </c>
+      <c r="E35">
+        <v>0.06618930140200975</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36">
+        <v>10</v>
+      </c>
       <c r="E36">
-        <v>0.03044603440401887</v>
+        <v>0.06017209218364523</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37">
+        <v>2</v>
+      </c>
+      <c r="E37">
+        <v>0.01203441843672905</v>
       </c>
     </row>
   </sheetData>

</xml_diff>